<commit_message>
Updated project with new changes
</commit_message>
<xml_diff>
--- a/downloads/daily_allocations.xlsx
+++ b/downloads/daily_allocations.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>id</t>
   </si>
@@ -43,34 +43,46 @@
     <t>station</t>
   </si>
   <si>
-    <t>operator</t>
+    <t>operator_name</t>
+  </si>
+  <si>
+    <t>operator_code</t>
+  </si>
+  <si>
+    <t>Shift 2</t>
   </si>
   <si>
     <t>Shift 1</t>
   </si>
   <si>
+    <t>7 AM</t>
+  </si>
+  <si>
+    <t>9 AM</t>
+  </si>
+  <si>
+    <t>6 AM</t>
+  </si>
+  <si>
     <t>8 AM</t>
   </si>
   <si>
-    <t>5:45  AM</t>
-  </si>
-  <si>
-    <t>4 AM</t>
-  </si>
-  <si>
-    <t>dw</t>
-  </si>
-  <si>
-    <t>Body Shop</t>
-  </si>
-  <si>
-    <t>Station 1</t>
-  </si>
-  <si>
-    <t>Worker 102 (102)</t>
-  </si>
-  <si>
-    <t>Worker 101 (101)</t>
+    <t>dh</t>
+  </si>
+  <si>
+    <t>Assembly</t>
+  </si>
+  <si>
+    <t>Pre-Assembly</t>
+  </si>
+  <si>
+    <t>Pre Line 1</t>
+  </si>
+  <si>
+    <t>Worker A1</t>
+  </si>
+  <si>
+    <t>401</t>
   </si>
 </sst>
 </file>
@@ -432,13 +444,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,63 +481,78 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>45968</v>
+        <v>45971</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>45968</v>
+        <v>45971</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
       </c>
       <c r="I3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="J3" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>